<commit_message>
Added 'password' to ERD & Schema
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Frank Eslami, CS 340-400</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>primary_user</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -135,15 +138,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,7 +1099,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1115,12 +1117,12 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
@@ -1128,19 +1130,21 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="C9" t="s">
@@ -1148,22 +1152,22 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1173,13 +1177,13 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1189,19 +1193,19 @@
       </c>
     </row>
     <row r="18" spans="3:7">
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1211,10 +1215,10 @@
       </c>
     </row>
     <row r="22" spans="3:7">
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added date_registered to ERD & Schema
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Frank Eslami, CS 340-400</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>date_registered</t>
   </si>
 </sst>
 </file>
@@ -1099,13 +1102,14 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1144,6 +1148,9 @@
       </c>
       <c r="G6" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>

<commit_message>
Added DOB to all files, including ERD & SCHEMA
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -82,7 +82,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>date_registered</t>
+    <t>DOB</t>
   </si>
 </sst>
 </file>
@@ -1102,14 +1102,13 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>

<commit_message>
ERD & Schema - added images table
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Frank Eslami, CS 340-400</t>
   </si>
@@ -70,19 +70,16 @@
     <t>id_friend</t>
   </si>
   <si>
-    <t>Permit</t>
-  </si>
-  <si>
-    <t>guest_user</t>
-  </si>
-  <si>
-    <t>primary_user</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>DOB</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>topic</t>
   </si>
 </sst>
 </file>
@@ -207,15 +204,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>400052</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:rowOff>9528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>400054</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114304</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -223,53 +220,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="2371727" y="4391023"/>
-          <a:ext cx="381001" cy="2"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>608807</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>795</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Connector 17"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="-1134269" y="2819401"/>
-          <a:ext cx="3496470" cy="10318"/>
+        <a:xfrm rot="5400000">
+          <a:off x="2433638" y="4348165"/>
+          <a:ext cx="295276" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -300,6 +253,50 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="-1057275" y="2733675"/>
+          <a:ext cx="3333750" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -432,107 +429,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>20638</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Straight Arrow Connector 29"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="609601" y="4400550"/>
-          <a:ext cx="1076325" cy="1588"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Straight Connector 33"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="609601" y="4572001"/>
-          <a:ext cx="1952625" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>332582</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>793</xdr:rowOff>
+      <xdr:colOff>332584</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>334170</xdr:colOff>
+      <xdr:colOff>342901</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>10318</xdr:rowOff>
+      <xdr:rowOff>10319</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -541,8 +447,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="4843463" y="2386012"/>
-          <a:ext cx="962025" cy="1588"/>
+          <a:off x="5061747" y="2595565"/>
+          <a:ext cx="534191" cy="10317"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -766,6 +672,983 @@
         <a:xfrm rot="5400000" flipH="1" flipV="1">
           <a:off x="1600200" y="1238250"/>
           <a:ext cx="228600" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="609601" y="4391025"/>
+          <a:ext cx="1076325" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>115888</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2581275" y="4495800"/>
+          <a:ext cx="942975" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>11</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5600705" y="3638555"/>
+          <a:ext cx="1181090" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1905000" y="3038476"/>
+          <a:ext cx="4286250" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685007</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>181768</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>686595</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1804988" y="3138487"/>
+          <a:ext cx="200025" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523082</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>10318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>524670</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>793</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3348038" y="4481512"/>
+          <a:ext cx="561975" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>125413</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Straight Connector 61"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762375" y="4505325"/>
+          <a:ext cx="2419350" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28573</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Arc 71"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19728593" flipH="1" flipV="1">
+          <a:off x="3457575" y="4219573"/>
+          <a:ext cx="457200" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 21521811"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Connector 72"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3609975" y="4752975"/>
+          <a:ext cx="3105150" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>277020</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Connector 76"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5863432" y="3348038"/>
+          <a:ext cx="1704181" cy="794"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Straight Arrow Connector 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5324476" y="2486025"/>
+          <a:ext cx="1400175" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647701</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>181769</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>648498</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161928</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="Straight Connector 82"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4610895" y="4267200"/>
+          <a:ext cx="170659" cy="797"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>274677</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28129</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586255</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>134804</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Arc 87"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="11055407" flipH="1" flipV="1">
+          <a:off x="5989677" y="4219129"/>
+          <a:ext cx="311578" cy="297175"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17284485"/>
+            <a:gd name="adj2" fmla="val 4103051"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Straight Connector 89"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4686300" y="4362450"/>
+          <a:ext cx="2562225" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>65127</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9079</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>376705</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>115754</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="Arc 93"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="11055407" flipH="1" flipV="1">
+          <a:off x="6504027" y="4200079"/>
+          <a:ext cx="311578" cy="297175"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17284485"/>
+            <a:gd name="adj2" fmla="val 4103051"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>267494</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>96046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276228</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="Straight Connector 94"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="6568284" y="4615656"/>
+          <a:ext cx="284954" cy="8734"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190503</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200028</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Straight Connector 97"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="6153153" y="3286125"/>
+          <a:ext cx="2181226" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190503</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96840</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="100" name="Straight Connector 99"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1971676" y="2190750"/>
+          <a:ext cx="5267327" cy="1590"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217527</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>151953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>529105</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68128</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="Arc 102"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5208627" y="2056953"/>
+          <a:ext cx="311578" cy="297175"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17284485"/>
+            <a:gd name="adj2" fmla="val 4103051"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314327</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314328</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="Straight Connector 103"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5214941" y="1995488"/>
+          <a:ext cx="180974" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>751682</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="Straight Arrow Connector 108"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="1832769" y="2052638"/>
+          <a:ext cx="277019" cy="794"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1101,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,10 +2029,10 @@
         <v>7</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1217,15 +2100,21 @@
     </row>
     <row r="21" spans="3:7">
       <c r="C21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Add Quote' HTML layout, less images. Next - store into database.
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Frank Eslami, CS 340-400</t>
   </si>
@@ -61,9 +61,6 @@
     <t>id_topic</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>Friends</t>
   </si>
   <si>
@@ -80,6 +77,12 @@
   </si>
   <si>
     <t>topic</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>id_image</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -146,6 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,13 +165,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>465932</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>10318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>467520</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19843</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -205,13 +209,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>9528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>114304</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -249,13 +253,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -293,13 +297,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>125413</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -340,13 +344,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>10317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>324647</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -384,13 +388,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -431,13 +435,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>332584</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>47628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>10319</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -475,13 +479,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>11113</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -519,13 +523,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>380206</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>162719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>381794</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>10319</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -564,15 +568,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342107</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361156</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>10319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>343695</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>362744</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>794</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -582,7 +586,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="5872163" y="1528763"/>
+          <a:off x="5167312" y="1528763"/>
           <a:ext cx="371475" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -610,13 +614,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>11113</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -627,7 +631,7 @@
       <xdr:spPr>
         <a:xfrm rot="10800000">
           <a:off x="1714500" y="1343025"/>
-          <a:ext cx="4343400" cy="1588"/>
+          <a:ext cx="3638550" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -654,13 +658,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>494506</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>172244</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>496094</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>19844</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -701,13 +705,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>11113</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -745,13 +749,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>115888</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -789,13 +793,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>11</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -833,13 +837,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -877,13 +881,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>685007</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>181768</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>686595</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -924,13 +928,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>523082</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>10318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>524670</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>793</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -968,13 +972,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>125413</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1012,13 +1016,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>28573</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>161923</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1067,13 +1071,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1111,13 +1115,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>19844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>277020</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1155,13 +1159,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>285751</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>11113</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1202,13 +1206,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>647701</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>181769</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>648498</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161928</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1246,13 +1250,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>274677</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>28129</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>586255</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>134804</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1301,13 +1305,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1345,13 +1349,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>65127</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>9079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>376705</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>115754</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1400,13 +1404,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>267494</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>96046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>276228</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1444,13 +1448,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>190503</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200028</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1488,13 +1492,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752476</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>190503</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1532,13 +1536,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>217527</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>151953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>529105</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>68128</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1587,13 +1591,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>314327</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>314328</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1631,13 +1635,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>751682</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752476</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>96044</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1649,6 +1653,273 @@
         <a:xfrm rot="5400000" flipH="1" flipV="1">
           <a:off x="1832769" y="2052638"/>
           <a:ext cx="277019" cy="794"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361157</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>362745</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>794</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5891213" y="2290763"/>
+          <a:ext cx="371475" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361952</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6076952" y="2085978"/>
+          <a:ext cx="971548" cy="9523"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608807</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Connector 46"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="6661945" y="1719262"/>
+          <a:ext cx="772320" cy="796"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1588</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Connector 50"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1971675" y="1333500"/>
+          <a:ext cx="5086350" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>484982</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>485778</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>795</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Connector 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="8366920" y="947737"/>
+          <a:ext cx="772320" cy="796"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>761206</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>162719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>762794</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>10319</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="1866900" y="1228725"/>
+          <a:ext cx="228600" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1982,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2012,108 +2283,119 @@
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="C6" s="1" t="s">
-        <v>4</v>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="C9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="C13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
+      <c r="G14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="3:7">
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="21" spans="3:7">
       <c r="C21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="1" t="s">
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Next - get quotes from database
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Frank Eslami, CS 340-400</t>
   </si>
@@ -79,10 +79,13 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Images</t>
+    <t>Relationship</t>
   </si>
   <si>
-    <t>id_image</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>id_relation</t>
   </si>
 </sst>
 </file>
@@ -141,15 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2256,7 +2260,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2274,12 +2278,12 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
@@ -2288,10 +2292,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2340,9 +2344,7 @@
       <c r="G14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H14" s="6"/>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
@@ -2356,7 +2358,7 @@
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="21" spans="3:7">
       <c r="C21" t="s">

</xml_diff>